<commit_message>
Relation et medicaments virtuels (#83) 95109953554694cc84bdafe7f3b17f6fb9b2b069
</commit_message>
<xml_diff>
--- a/main/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/main/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -83,12 +83,15 @@
     <sheet name="Mapping Table 73" r:id="rId77" sheetId="75"/>
     <sheet name="Mapping Table 74" r:id="rId78" sheetId="76"/>
     <sheet name="Mapping Table 75" r:id="rId79" sheetId="77"/>
+    <sheet name="Mapping Table 76" r:id="rId80" sheetId="78"/>
+    <sheet name="Mapping Table 77" r:id="rId81" sheetId="79"/>
+    <sheet name="Mapping Table 78" r:id="rId82" sheetId="80"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="99">
   <si>
     <t>Property</t>
   </si>
@@ -132,7 +135,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-05T10:03:44+00:00</t>
+    <t>2025-07-09T18:07:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1062,6 +1065,62 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1129,7 +1188,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1185,7 +1244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1225,6 +1284,62 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
         <v>60</v>
       </c>
       <c r="B3" s="2"/>
@@ -1241,7 +1356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1281,62 +1396,6 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
         <v>60</v>
       </c>
       <c r="B3" s="2"/>
@@ -1353,7 +1412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1422,7 +1481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1491,7 +1550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1560,7 +1619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1629,7 +1688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1685,7 +1744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1741,7 +1800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1797,7 +1856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1866,7 +1925,89 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1935,89 +2076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2073,7 +2132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2129,7 +2188,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2185,7 +2244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2254,7 +2313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2323,7 +2382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2379,7 +2438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2435,7 +2494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2491,7 +2550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2560,7 +2619,141 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2629,141 +2822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2819,7 +2878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2875,7 +2934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2931,7 +2990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3000,7 +3059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3069,7 +3128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3125,7 +3184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3181,7 +3240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3237,7 +3296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3306,7 +3365,76 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3375,76 +3503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3500,7 +3559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3556,7 +3615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3612,7 +3671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3681,7 +3740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3750,7 +3809,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3806,7 +3865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3862,7 +3921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3918,7 +3977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3987,7 +4046,141 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -4056,141 +4249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -4259,7 +4318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -4350,7 +4409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -4458,7 +4517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -4514,7 +4573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -4570,7 +4629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -4626,7 +4685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -4851,7 +4910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -4905,7 +4964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -4959,7 +5018,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -5002,63 +5117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -5101,7 +5160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -5183,7 +5242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -5252,7 +5311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -5325,7 +5384,7 @@
         <v>39</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -5338,7 +5397,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -5351,7 +5410,7 @@
         <v>39</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -5399,7 +5458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -5446,7 +5505,7 @@
         <v>39</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -5459,7 +5518,7 @@
         <v>39</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -5472,7 +5531,7 @@
         <v>39</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -5520,7 +5579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -5619,7 +5678,7 @@
         <v>39</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -5632,7 +5691,7 @@
         <v>39</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -5645,7 +5704,7 @@
         <v>39</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -5771,7 +5830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -5818,7 +5877,7 @@
         <v>39</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -5831,7 +5890,7 @@
         <v>39</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -5844,7 +5903,7 @@
         <v>39</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -5957,9 +6016,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6032,62 +6091,204 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" t="s" s="2">
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s" s="2">
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D3" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="2">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s" s="2">
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="2">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" t="s" s="2">
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D9" t="s" s="2">
+      <c r="D5" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="E5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -6127,7 +6328,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -6141,60 +6342,4 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>